<commit_message>
DDF working as it should needs inhansement and refinement
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="17400" windowHeight="6440"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="17400" windowHeight="6440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
@@ -420,7 +420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -507,7 +507,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -524,7 +524,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -541,7 +541,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>